<commit_message>
feat: add dtaa for first courses of 2025
</commit_message>
<xml_diff>
--- a/data/formations-suivi-inscriptions.xlsx
+++ b/data/formations-suivi-inscriptions.xlsx
@@ -133,7 +133,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf fontId="1" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -154,6 +154,9 @@
     </xf>
     <xf fontId="1" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1">
       <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="1" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -799,20 +802,18 @@
     </row>
     <row r="8" ht="14.25">
       <c r="A8" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C8" s="2">
-        <v>2022</v>
+        <v>2025</v>
       </c>
       <c r="D8" s="7">
-        <v>150</v>
-      </c>
-      <c r="E8" s="3">
-        <v>55</v>
-      </c>
+        <v>250</v>
+      </c>
+      <c r="E8" s="3"/>
     </row>
     <row r="9" ht="14.25">
       <c r="A9" s="1" t="s">
@@ -822,13 +823,13 @@
         <v>8</v>
       </c>
       <c r="C9" s="2">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="D9" s="7">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="E9" s="3">
-        <v>35</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" ht="14.25">
@@ -839,13 +840,13 @@
         <v>8</v>
       </c>
       <c r="C10" s="2">
-        <v>2024</v>
+        <v>2023</v>
       </c>
       <c r="D10" s="7">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="E10" s="3">
-        <v>47</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" ht="14.25">
@@ -856,30 +857,30 @@
         <v>8</v>
       </c>
       <c r="C11" s="2">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="D11" s="7">
-        <v>250</v>
+        <v>150</v>
       </c>
       <c r="E11" s="3">
-        <v>27</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" ht="14.25">
       <c r="A12" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C12" s="2">
-        <v>2022</v>
+        <v>2025</v>
       </c>
       <c r="D12" s="7">
-        <v>350</v>
+        <v>250</v>
       </c>
       <c r="E12" s="3">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" ht="14.25">
@@ -890,13 +891,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="2">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="D13" s="7">
-        <v>150</v>
+        <v>350</v>
       </c>
       <c r="E13" s="3">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" ht="14.25">
@@ -907,21 +908,21 @@
         <v>10</v>
       </c>
       <c r="C14" s="2">
-        <v>2024</v>
+        <v>2023</v>
       </c>
       <c r="D14" s="7">
         <v>150</v>
       </c>
       <c r="E14" s="3">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" ht="14.25">
       <c r="A15" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C15" s="2">
         <v>2024</v>
@@ -930,15 +931,15 @@
         <v>150</v>
       </c>
       <c r="E15" s="3">
-        <v>46</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" ht="14.25">
       <c r="A16" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>12</v>
+        <v>9</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="C16" s="2">
         <v>2025</v>
@@ -946,16 +947,14 @@
       <c r="D16" s="7">
         <v>250</v>
       </c>
-      <c r="E16" s="3">
-        <v>34</v>
-      </c>
+      <c r="E16" s="3"/>
     </row>
     <row r="17" ht="14.25">
       <c r="A17" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C17" s="2">
         <v>2024</v>
@@ -964,15 +963,15 @@
         <v>150</v>
       </c>
       <c r="E17" s="3">
-        <v>32</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" ht="14.25">
       <c r="A18" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>12</v>
       </c>
       <c r="C18" s="2">
         <v>2025</v>
@@ -980,13 +979,62 @@
       <c r="D18" s="7">
         <v>250</v>
       </c>
+      <c r="E18" s="3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" ht="14.25">
+      <c r="A19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="2">
+        <v>2024</v>
+      </c>
+      <c r="D19" s="7">
+        <v>150</v>
+      </c>
+      <c r="E19" s="3">
+        <v>32</v>
+      </c>
     </row>
     <row r="20" ht="14.25">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="3"/>
+      <c r="A20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="2">
+        <v>2025</v>
+      </c>
+      <c r="D20" s="7">
+        <v>250</v>
+      </c>
+      <c r="E20" s="9"/>
+    </row>
+    <row r="21" ht="14.25">
+      <c r="A21" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" s="2">
+        <v>2025</v>
+      </c>
+      <c r="D21" s="7">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="23" ht="14.25">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>

</xml_diff>